<commit_message>
* Removed copies of used kernels in latex/code folter. * Added thesis namespace and copied selected algorithms there * Beautified selected kernels which led to fewer instructions in most cases * Rerun benchmarks for thesis algorithms, recreated charts and performance counters
</commit_message>
<xml_diff>
--- a/latex/tables/performance_counter.xlsx
+++ b/latex/tables/performance_counter.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="405" windowWidth="20835" windowHeight="8475"/>
+    <workbookView xWindow="720" yWindow="315" windowWidth="27555" windowHeight="13065"/>
   </bookViews>
   <sheets>
-    <sheet name="Jul-11-2013_15-48-16" sheetId="1" r:id="rId1"/>
+    <sheet name="Jul-17-2013_13-37-23" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Method</t>
   </si>
@@ -25,6 +25,9 @@
     <t xml:space="preserve"> WorkGroupSize</t>
   </si>
   <si>
+    <t xml:space="preserve"> Time</t>
+  </si>
+  <si>
     <t xml:space="preserve"> LocalMemSize</t>
   </si>
   <si>
@@ -61,46 +64,55 @@
     <t xml:space="preserve"> FetchSize</t>
   </si>
   <si>
+    <t xml:space="preserve"> CacheHit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FetchUnitBusy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FetchUnitStalled</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WriteUnitStalled</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FastPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CompletePath</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PathUtilization</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LDSBankConflict</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {   4000    4000       1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {   16    16     1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {   1008    1008       1}</t>
+  </si>
+  <si>
     <t>Mult</t>
   </si>
   <si>
+    <t>MultLocal</t>
+  </si>
+  <si>
+    <t>MultBlock</t>
+  </si>
+  <si>
     <t>MultBlockLocal</t>
-  </si>
-  <si>
-    <t>MultBlock</t>
-  </si>
-  <si>
-    <t>MultLocal</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Time (ms)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CacheHit (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FetchUnitBusy (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {  4000  4000  }</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {  1008  1008  }</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {  16  16  }</t>
-  </si>
-  <si>
-    <t>Occupancy (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -579,10 +591,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -925,36 +936,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,66 +981,81 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
       <c r="D2">
-        <v>14387</v>
+        <v>14390.26533</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1033,224 +1064,284 @@
         <v>6</v>
       </c>
       <c r="G2">
+        <v>84000</v>
+      </c>
+      <c r="H2">
+        <v>20019</v>
+      </c>
+      <c r="I2">
+        <v>8000</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>62.48</v>
+      </c>
+      <c r="N2">
+        <v>2.5</v>
+      </c>
+      <c r="O2">
+        <v>35.99</v>
+      </c>
+      <c r="P2">
+        <v>23149004.75</v>
+      </c>
+      <c r="Q2">
+        <v>57.52</v>
+      </c>
+      <c r="R2">
+        <v>99.87</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>21000</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
         <v>100</v>
       </c>
-      <c r="H2">
-        <v>84000</v>
-      </c>
-      <c r="I2">
-        <v>20019</v>
-      </c>
-      <c r="J2">
-        <v>8000</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>62.48</v>
-      </c>
-      <c r="O2" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="P2" s="2">
-        <v>35.99</v>
-      </c>
-      <c r="Q2">
-        <v>23002707</v>
-      </c>
-      <c r="R2" s="2">
-        <v>57.58</v>
-      </c>
-      <c r="S2" s="2">
-        <v>99.87</v>
+      <c r="X2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3">
-        <v>5364</v>
+        <v>5131.8321100000003</v>
       </c>
       <c r="E3">
         <v>2048</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G3">
+        <v>84000</v>
+      </c>
+      <c r="H3">
+        <v>7767</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>4000</v>
+      </c>
+      <c r="L3">
+        <v>500</v>
+      </c>
+      <c r="M3">
+        <v>68.05</v>
+      </c>
+      <c r="N3">
+        <v>15.53</v>
+      </c>
+      <c r="O3">
+        <v>59.3</v>
+      </c>
+      <c r="P3">
+        <v>9729495.1300000008</v>
+      </c>
+      <c r="Q3">
+        <v>7.34</v>
+      </c>
+      <c r="R3">
+        <v>17.52</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>21000</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
         <v>100</v>
       </c>
-      <c r="H3">
-        <v>84000</v>
-      </c>
-      <c r="I3">
-        <v>8516</v>
-      </c>
-      <c r="J3">
-        <v>500</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>4250</v>
-      </c>
-      <c r="M3">
-        <v>500</v>
-      </c>
-      <c r="N3" s="2">
-        <v>71.319999999999993</v>
-      </c>
-      <c r="O3" s="2">
-        <v>17.03</v>
-      </c>
-      <c r="P3" s="2">
-        <v>61.13</v>
-      </c>
-      <c r="Q3">
-        <v>10095104</v>
-      </c>
-      <c r="R3" s="2">
-        <v>3.85</v>
-      </c>
-      <c r="S3" s="2">
-        <v>16.75</v>
+      <c r="X3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>1101</v>
+        <v>1074.0791099999999</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>37.5</v>
+        <v>15914</v>
       </c>
       <c r="H4">
-        <v>15876</v>
+        <v>23782.45</v>
       </c>
       <c r="I4">
-        <v>28796</v>
+        <v>7917.56</v>
       </c>
       <c r="J4">
-        <v>7937</v>
+        <v>3.96</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
-        <v>74.55</v>
-      </c>
-      <c r="O4" s="2">
-        <v>3.63</v>
-      </c>
-      <c r="P4" s="2">
-        <v>77.91</v>
+        <v>62.79</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>84.12</v>
+      </c>
+      <c r="P4">
+        <v>21510158.309999999</v>
       </c>
       <c r="Q4">
-        <v>21983484</v>
-      </c>
-      <c r="R4" s="2">
-        <v>29.73</v>
-      </c>
-      <c r="S4" s="2">
-        <v>99.06</v>
+        <v>31.23</v>
+      </c>
+      <c r="R4">
+        <v>99.39</v>
+      </c>
+      <c r="S4">
+        <v>16.48</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>62500</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>100</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5">
-        <v>1839</v>
+        <v>1823.73711</v>
       </c>
       <c r="E5">
         <v>32768</v>
       </c>
       <c r="F5">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G5">
-        <v>12.5</v>
+        <v>15914</v>
       </c>
       <c r="H5">
-        <v>15876</v>
+        <v>44214.18</v>
       </c>
       <c r="I5">
-        <v>45008</v>
+        <v>502.8</v>
       </c>
       <c r="J5">
-        <v>504</v>
+        <v>3.99</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>18352.07</v>
       </c>
       <c r="L5">
-        <v>18459</v>
+        <v>2011.19</v>
       </c>
       <c r="M5">
-        <v>2016</v>
-      </c>
-      <c r="N5" s="2">
-        <v>69.790000000000006</v>
-      </c>
-      <c r="O5" s="2">
-        <v>89.3</v>
-      </c>
-      <c r="P5" s="2">
-        <v>75.88</v>
+        <v>69.55</v>
+      </c>
+      <c r="N5">
+        <v>87.94</v>
+      </c>
+      <c r="O5">
+        <v>76.69</v>
+      </c>
+      <c r="P5">
+        <v>5030125.5599999996</v>
       </c>
       <c r="Q5">
-        <v>4918471</v>
-      </c>
-      <c r="R5" s="2">
-        <v>38.53</v>
-      </c>
-      <c r="S5" s="2">
-        <v>4.18</v>
+        <v>37.14</v>
+      </c>
+      <c r="R5">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="S5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="T5">
+        <v>0.08</v>
+      </c>
+      <c r="U5">
+        <v>63508.5</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>100</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>